<commit_message>
EFOGC-4683 added Campaign substate form and TestCampaignSubstateForm class, updated Regression test plan sheet and updated regression-suite.xml
</commit_message>
<xml_diff>
--- a/src/test/resources/Regression/testplan/exccel/E4O_Regression_Test_Plan.xlsx
+++ b/src/test/resources/Regression/testplan/exccel/E4O_Regression_Test_Plan.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="325">
   <si>
     <t>TestCase ID</t>
   </si>
@@ -964,6 +964,33 @@
   </si>
   <si>
     <t>1. edit an existing product type and edit an existing characteristic to add more values in list type characteristic</t>
+  </si>
+  <si>
+    <t>UC09-01</t>
+  </si>
+  <si>
+    <t>UC09-02</t>
+  </si>
+  <si>
+    <t>UC09-03</t>
+  </si>
+  <si>
+    <t>create Campaign substate under Adminstration section</t>
+  </si>
+  <si>
+    <t>Delete the already exisiting campaign substate</t>
+  </si>
+  <si>
+    <t>Edit the already exisitng campaign substate</t>
+  </si>
+  <si>
+    <t>Campaign substate created successfully and verified on UI</t>
+  </si>
+  <si>
+    <t>Campaign substate edited successfully and verified on UI.</t>
+  </si>
+  <si>
+    <t>Campaign substate deleted successfully and verified on UI.</t>
   </si>
 </sst>
 </file>
@@ -1055,7 +1082,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -1063,43 +1090,61 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1416,8 +1461,8 @@
     <col min="7" max="7" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="18" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:3" s="8" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1432,146 +1477,146 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+    <row r="3" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+    <row r="4" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+    <row r="8" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+    <row r="9" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
+    <row r="10" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+    <row r="11" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+    <row r="12" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
+    <row r="13" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
+    <row r="14" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
+    <row r="15" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="4" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1675,68 +1720,68 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
+      <c r="A25" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="3" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
+      <c r="A26" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C26" s="3" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
+      <c r="A27" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="3" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
+      <c r="A28" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="C28" s="3" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
+      <c r="A29" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="C29" s="3" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
+      <c r="A30" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="C30" s="3" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1784,25 +1829,25 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="6" t="s">
+    <row r="35" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="B35" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C35" s="6" t="s">
+      <c r="C35" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="6" t="s">
+    <row r="36" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="B36" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C36" s="6" t="s">
+      <c r="C36" s="3" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1852,1025 +1897,1071 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E71"/>
+  <dimension ref="A1:E74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" customWidth="1"/>
-    <col min="3" max="3" width="66.28515625" customWidth="1"/>
-    <col min="4" max="4" width="23.42578125" customWidth="1"/>
-    <col min="5" max="5" width="32.28515625" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" style="14" customWidth="1"/>
+    <col min="3" max="3" width="66.28515625" style="14" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" style="14" customWidth="1"/>
+    <col min="5" max="5" width="32.28515625" style="14" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="11" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="12" t="s">
         <v>248</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="12" t="s">
         <v>249</v>
       </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="4" t="s">
+      <c r="D2" s="13"/>
+      <c r="E2" s="12" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="12" t="s">
         <v>251</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="12" t="s">
         <v>252</v>
       </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="4" t="s">
+      <c r="D3" s="13"/>
+      <c r="E3" s="12" t="s">
         <v>253</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="12" t="s">
         <v>257</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="12" t="s">
         <v>258</v>
       </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="4" t="s">
+      <c r="D4" s="13"/>
+      <c r="E4" s="12" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="12" t="s">
         <v>260</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="12" t="s">
         <v>261</v>
       </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="4" t="s">
+      <c r="D5" s="13"/>
+      <c r="E5" s="12" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="12" t="s">
         <v>263</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="12" t="s">
         <v>264</v>
       </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="4" t="s">
+      <c r="D6" s="13"/>
+      <c r="E6" s="12" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="12" t="s">
         <v>254</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="12" t="s">
         <v>255</v>
       </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="4" t="s">
+      <c r="D7" s="13"/>
+      <c r="E7" s="12" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
+    <row r="8" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
         <v>295</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="15" t="s">
         <v>296</v>
       </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="12" t="s">
+      <c r="D8" s="16"/>
+      <c r="E8" s="15" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
+    <row r="9" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
         <v>298</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="15" t="s">
         <v>299</v>
       </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="12" t="s">
+      <c r="D9" s="16"/>
+      <c r="E9" s="15" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
+    <row r="10" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
         <v>301</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="15" t="s">
         <v>302</v>
       </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="12" t="s">
+      <c r="D10" s="16"/>
+      <c r="E10" s="15" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
+    <row r="11" spans="1:5" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
         <v>304</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="15" t="s">
         <v>305</v>
       </c>
-      <c r="D11" s="13"/>
-      <c r="E11" s="12" t="s">
+      <c r="D11" s="16"/>
+      <c r="E11" s="15" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
+    <row r="12" spans="1:5" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
         <v>266</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="9" t="s">
         <v>267</v>
       </c>
-      <c r="D12" s="15"/>
-      <c r="E12" s="14" t="s">
+      <c r="D12" s="10"/>
+      <c r="E12" s="9" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
+    <row r="13" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
         <v>269</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="9" t="s">
         <v>293</v>
       </c>
-      <c r="D13" s="15"/>
-      <c r="E13" s="14" t="s">
+      <c r="D13" s="10"/>
+      <c r="E13" s="9" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
+    <row r="14" spans="1:5" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
         <v>285</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="9" t="s">
         <v>307</v>
       </c>
-      <c r="D14" s="15"/>
-      <c r="E14" s="14" t="s">
+      <c r="D14" s="10"/>
+      <c r="E14" s="9" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
+    <row r="15" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
         <v>286</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="9" t="s">
         <v>309</v>
       </c>
-      <c r="D15" s="15"/>
-      <c r="E15" s="14" t="s">
+      <c r="D15" s="10"/>
+      <c r="E15" s="9" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="s">
+    <row r="16" spans="1:5" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
         <v>287</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="9" t="s">
         <v>288</v>
       </c>
-      <c r="D16" s="15"/>
-      <c r="E16" s="14" t="s">
+      <c r="D16" s="10"/>
+      <c r="E16" s="9" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="s">
+    <row r="17" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
         <v>290</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="9" t="s">
         <v>291</v>
       </c>
-      <c r="D17" s="15"/>
-      <c r="E17" s="14" t="s">
+      <c r="D17" s="10"/>
+      <c r="E17" s="9" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+    <row r="18" spans="1:5" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>316</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>319</v>
+      </c>
+      <c r="D18" s="10"/>
+      <c r="E18" s="9" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>321</v>
+      </c>
+      <c r="D19" s="10"/>
+      <c r="E19" s="9" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>318</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>320</v>
+      </c>
+      <c r="D20" s="10"/>
+      <c r="E20" s="9" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="12" t="s">
         <v>270</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B21" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C21" s="12" t="s">
         <v>271</v>
       </c>
-      <c r="D18" s="5"/>
-      <c r="E18" s="4" t="s">
+      <c r="D21" s="13"/>
+      <c r="E21" s="12" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+    <row r="22" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="12" t="s">
         <v>273</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B22" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C22" s="12" t="s">
         <v>274</v>
       </c>
-      <c r="D19" s="5"/>
-      <c r="E19" s="4" t="s">
+      <c r="D22" s="13"/>
+      <c r="E22" s="12" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
+    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="12" t="s">
         <v>276</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B23" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C23" s="12" t="s">
         <v>277</v>
       </c>
-      <c r="D20" s="5"/>
-      <c r="E20" s="4" t="s">
+      <c r="D23" s="13"/>
+      <c r="E23" s="12" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="21" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+    <row r="24" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="19" t="s">
         <v>224</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B24" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C24" s="19" t="s">
         <v>225</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="E24" s="19" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="22" spans="1:5" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+    <row r="25" spans="1:5" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="19" t="s">
         <v>227</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B25" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C25" s="19" t="s">
         <v>246</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="E25" s="19" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="23" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
+    <row r="26" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="20" t="s">
         <v>103</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B26" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C26" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="E23" s="7" t="s">
+      <c r="E26" s="20" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="24" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
+    <row r="27" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="20" t="s">
         <v>132</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B27" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="C27" s="20" t="s">
         <v>279</v>
       </c>
-      <c r="E24" s="7" t="s">
+      <c r="E27" s="20" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="25" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
+    <row r="28" spans="1:5" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="20" t="s">
         <v>281</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B28" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="C28" s="20" t="s">
         <v>282</v>
       </c>
-      <c r="E25" s="7" t="s">
+      <c r="E28" s="20" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="26" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
+    <row r="29" spans="1:5" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B29" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C29" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="E26" s="7" t="s">
+      <c r="E29" s="20" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="27" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="7" t="s">
+    <row r="30" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="20" t="s">
         <v>133</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="B30" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="C30" s="20" t="s">
         <v>134</v>
       </c>
-      <c r="E27" s="7" t="s">
+      <c r="E30" s="20" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="28" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="7" t="s">
+    <row r="31" spans="1:5" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="20" t="s">
         <v>136</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="B31" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="C28" s="7" t="s">
+      <c r="C31" s="20" t="s">
         <v>284</v>
       </c>
-      <c r="E28" s="7" t="s">
+      <c r="E31" s="20" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="29" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="17" t="s">
+    <row r="32" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="B29" s="17" t="s">
+      <c r="B32" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="C29" s="17" t="s">
+      <c r="C32" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="E29" s="17" t="s">
+      <c r="E32" s="21" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="30" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="17" t="s">
+    <row r="33" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="B30" s="17" t="s">
+      <c r="B33" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="C30" s="17" t="s">
+      <c r="C33" s="21" t="s">
         <v>139</v>
       </c>
-      <c r="E30" s="17" t="s">
+      <c r="E33" s="21" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="31" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="17" t="s">
+    <row r="34" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="21" t="s">
         <v>141</v>
       </c>
-      <c r="B31" s="17" t="s">
+      <c r="B34" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="C31" s="17" t="s">
+      <c r="C34" s="21" t="s">
         <v>142</v>
       </c>
-      <c r="E31" s="17" t="s">
+      <c r="E34" s="21" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="32" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="17" t="s">
+    <row r="35" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="B32" s="17" t="s">
+      <c r="B35" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="C32" s="17" t="s">
+      <c r="C35" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="E32" s="17" t="s">
+      <c r="E35" s="21" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="17" t="s">
+    <row r="36" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="21" t="s">
         <v>144</v>
       </c>
-      <c r="B33" s="17" t="s">
+      <c r="B36" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="C33" s="17" t="s">
+      <c r="C36" s="21" t="s">
         <v>311</v>
       </c>
-      <c r="E33" s="17" t="s">
+      <c r="E36" s="21" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="34" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="17" t="s">
+    <row r="37" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="21" t="s">
         <v>146</v>
       </c>
-      <c r="B34" s="17" t="s">
+      <c r="B37" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="C34" s="17" t="s">
+      <c r="C37" s="21" t="s">
         <v>147</v>
       </c>
-      <c r="E34" s="17" t="s">
+      <c r="E37" s="21" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="35" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="17" t="s">
+    <row r="38" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="21" t="s">
         <v>312</v>
       </c>
-      <c r="B35" s="17" t="s">
+      <c r="B38" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="C35" s="17" t="s">
+      <c r="C38" s="21" t="s">
         <v>313</v>
       </c>
-      <c r="E35" s="17" t="s">
+      <c r="E38" s="21" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="36" spans="1:5" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="17" t="s">
+    <row r="39" spans="1:5" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="21" t="s">
         <v>314</v>
       </c>
-      <c r="B36" s="17" t="s">
+      <c r="B39" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="C36" s="17" t="s">
+      <c r="C39" s="21" t="s">
         <v>315</v>
       </c>
-      <c r="E36" s="17" t="s">
+      <c r="E39" s="21" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="37" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="7" t="s">
+    <row r="40" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="B37" s="7" t="s">
+      <c r="B40" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="C37" s="7" t="s">
+      <c r="C40" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="E37" s="7" t="s">
+      <c r="E40" s="20" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="38" spans="1:5" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A38" s="7" t="s">
+    <row r="41" spans="1:5" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A41" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="B38" s="7" t="s">
+      <c r="B41" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="C38" s="7" t="s">
+      <c r="C41" s="20" t="s">
         <v>118</v>
       </c>
-      <c r="E38" s="7" t="s">
+      <c r="E41" s="20" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="39" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="7" t="s">
+    <row r="42" spans="1:5" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="B39" s="7" t="s">
+      <c r="B42" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="C39" s="7" t="s">
+      <c r="C42" s="20" t="s">
         <v>120</v>
       </c>
-      <c r="E39" s="7" t="s">
+      <c r="E42" s="20" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="40" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="7" t="s">
+    <row r="43" spans="1:5" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="20" t="s">
         <v>122</v>
       </c>
-      <c r="B40" s="7" t="s">
+      <c r="B43" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="C40" s="7" t="s">
+      <c r="C43" s="20" t="s">
         <v>121</v>
       </c>
-      <c r="E40" s="7" t="s">
+      <c r="E43" s="20" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="41" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="7" t="s">
+    <row r="44" spans="1:5" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="20" t="s">
         <v>123</v>
       </c>
-      <c r="B41" s="7" t="s">
+      <c r="B44" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="C41" s="7" t="s">
+      <c r="C44" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="E41" s="7" t="s">
+      <c r="E44" s="20" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="42" spans="1:5" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A42" s="7" t="s">
+    <row r="45" spans="1:5" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A45" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="B42" s="7" t="s">
+      <c r="B45" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="C42" s="7" t="s">
+      <c r="C45" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="E42" s="7" t="s">
+      <c r="E45" s="20" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="43" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="7" t="s">
+    <row r="46" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="20" t="s">
         <v>152</v>
       </c>
-      <c r="B43" s="7" t="s">
+      <c r="B46" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="C43" s="7" t="s">
+      <c r="C46" s="20" t="s">
         <v>153</v>
       </c>
-      <c r="E43" s="7" t="s">
+      <c r="E46" s="20" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="44" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="7" t="s">
+    <row r="47" spans="1:5" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A47" s="20" t="s">
         <v>125</v>
       </c>
-      <c r="B44" s="6" t="s">
+      <c r="B47" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="C44" s="7" t="s">
+      <c r="C47" s="20" t="s">
         <v>128</v>
       </c>
-      <c r="E44" s="7" t="s">
+      <c r="E47" s="20" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="45" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="7" t="s">
+    <row r="48" spans="1:5" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A48" s="20" t="s">
         <v>127</v>
       </c>
-      <c r="B45" s="6" t="s">
+      <c r="B48" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="C45" s="7" t="s">
+      <c r="C48" s="20" t="s">
         <v>129</v>
       </c>
-      <c r="E45" s="7" t="s">
+      <c r="E48" s="20" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="46" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A46" s="7" t="s">
+    <row r="49" spans="1:5" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A49" s="20" t="s">
         <v>130</v>
       </c>
-      <c r="B46" s="6" t="s">
+      <c r="B49" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="C46" s="7" t="s">
+      <c r="C49" s="20" t="s">
         <v>162</v>
       </c>
-      <c r="E46" s="7" t="s">
+      <c r="E49" s="20" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="47" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A47" s="7" t="s">
+    <row r="50" spans="1:5" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A50" s="20" t="s">
         <v>130</v>
       </c>
-      <c r="B47" s="6" t="s">
+      <c r="B50" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="C47" s="7" t="s">
+      <c r="C50" s="20" t="s">
         <v>131</v>
       </c>
-      <c r="E47" s="7" t="s">
+      <c r="E50" s="20" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="48" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="7" t="s">
+    <row r="51" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="20" t="s">
         <v>155</v>
       </c>
-      <c r="B48" s="6" t="s">
+      <c r="B51" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="C48" s="7" t="s">
+      <c r="C51" s="20" t="s">
         <v>156</v>
       </c>
-      <c r="E48" s="7" t="s">
+      <c r="E51" s="20" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="49" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="7" t="s">
+    <row r="52" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="20" t="s">
         <v>158</v>
       </c>
-      <c r="B49" s="6" t="s">
+      <c r="B52" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="C49" s="7" t="s">
+      <c r="C52" s="20" t="s">
         <v>159</v>
       </c>
-      <c r="E49" s="7" t="s">
+      <c r="E52" s="20" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="50" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
+    <row r="53" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="19" t="s">
         <v>161</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="B53" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="C50" s="2" t="s">
+      <c r="C53" s="19" t="s">
         <v>164</v>
       </c>
-      <c r="E50" s="2" t="s">
+      <c r="E53" s="19" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="51" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
+    <row r="54" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="19" t="s">
         <v>170</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B54" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="C54" s="19" t="s">
         <v>166</v>
       </c>
-      <c r="E51" s="2" t="s">
+      <c r="E54" s="19" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="52" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
+    <row r="55" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="19" t="s">
         <v>171</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="B55" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="C52" s="2" t="s">
+      <c r="C55" s="19" t="s">
         <v>168</v>
       </c>
-      <c r="E52" s="2" t="s">
+      <c r="E55" s="19" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="53" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
+    <row r="56" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="19" t="s">
         <v>172</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="B56" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="C56" s="19" t="s">
         <v>174</v>
       </c>
-      <c r="E53" s="2" t="s">
+      <c r="E56" s="19" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="54" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
+    <row r="57" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="19" t="s">
         <v>176</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="B57" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="C54" s="2" t="s">
+      <c r="C57" s="19" t="s">
         <v>175</v>
       </c>
-      <c r="E54" s="2" t="s">
+      <c r="E57" s="19" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="55" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="2" t="s">
+    <row r="58" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="19" t="s">
         <v>181</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="B58" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="C55" s="2" t="s">
+      <c r="C58" s="19" t="s">
         <v>199</v>
       </c>
-      <c r="E55" s="2" t="s">
+      <c r="E58" s="19" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="56" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="2" t="s">
+    <row r="59" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="19" t="s">
         <v>184</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B59" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="C56" s="2" t="s">
+      <c r="C59" s="19" t="s">
         <v>182</v>
       </c>
-      <c r="E56" s="2" t="s">
+      <c r="E59" s="19" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="57" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="2" t="s">
+    <row r="60" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="19" t="s">
         <v>187</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B60" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="C57" s="2" t="s">
+      <c r="C60" s="19" t="s">
         <v>185</v>
       </c>
-      <c r="E57" s="2" t="s">
+      <c r="E60" s="19" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="58" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
+    <row r="61" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="19" t="s">
         <v>190</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="B61" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="C58" s="2" t="s">
+      <c r="C61" s="19" t="s">
         <v>188</v>
       </c>
-      <c r="E58" s="2" t="s">
+      <c r="E61" s="19" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="59" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="2" t="s">
+    <row r="62" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="19" t="s">
         <v>193</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="B62" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="C59" s="2" t="s">
+      <c r="C62" s="19" t="s">
         <v>191</v>
       </c>
-      <c r="E59" s="2" t="s">
+      <c r="E62" s="19" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="60" spans="1:5" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A60" s="2" t="s">
+    <row r="63" spans="1:5" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A63" s="19" t="s">
         <v>195</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="B63" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="C63" s="19" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="61" spans="1:5" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A61" s="2" t="s">
+    <row r="64" spans="1:5" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A64" s="19" t="s">
         <v>197</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="B64" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="C61" s="2" t="s">
+      <c r="C64" s="19" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="62" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="2" t="s">
+    <row r="65" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="19" t="s">
         <v>201</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="B65" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="C62" s="2" t="s">
+      <c r="C65" s="19" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="63" spans="1:5" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="2" t="s">
+    <row r="66" spans="1:5" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A66" s="19" t="s">
         <v>178</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="B66" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="C63" s="2" t="s">
+      <c r="C66" s="19" t="s">
         <v>179</v>
       </c>
-      <c r="E63" s="2" t="s">
+      <c r="E66" s="19" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="64" spans="1:5" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A64" s="2" t="s">
+    <row r="67" spans="1:5" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A67" s="19" t="s">
         <v>208</v>
       </c>
-      <c r="B64" s="2" t="s">
+      <c r="B67" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="C64" s="2" t="s">
+      <c r="C67" s="19" t="s">
         <v>209</v>
       </c>
-      <c r="E64" s="2" t="s">
+      <c r="E67" s="19" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="65" spans="1:5" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A65" s="2" t="s">
+    <row r="68" spans="1:5" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A68" s="19" t="s">
         <v>213</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="B68" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="C65" s="2" t="s">
+      <c r="C68" s="19" t="s">
         <v>214</v>
       </c>
-      <c r="E65" s="2" t="s">
+      <c r="E68" s="19" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="66" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A66" s="7" t="s">
+    <row r="69" spans="1:5" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A69" s="20" t="s">
         <v>202</v>
       </c>
-      <c r="B66" s="7" t="s">
+      <c r="B69" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="C66" s="7" t="s">
+      <c r="C69" s="20" t="s">
         <v>203</v>
       </c>
-      <c r="E66" s="7" t="s">
+      <c r="E69" s="20" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="67" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A67" s="7" t="s">
+    <row r="70" spans="1:5" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A70" s="20" t="s">
         <v>210</v>
       </c>
-      <c r="B67" s="7" t="s">
+      <c r="B70" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="C67" s="7" t="s">
+      <c r="C70" s="20" t="s">
         <v>211</v>
       </c>
-      <c r="E67" s="7" t="s">
+      <c r="E70" s="20" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="68" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A68" s="7" t="s">
+    <row r="71" spans="1:5" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A71" s="20" t="s">
         <v>210</v>
       </c>
-      <c r="B68" s="7" t="s">
+      <c r="B71" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="C68" s="7" t="s">
+      <c r="C71" s="20" t="s">
         <v>217</v>
       </c>
-      <c r="E68" s="7" t="s">
+      <c r="E71" s="20" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="69" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A69" s="7" t="s">
+    <row r="72" spans="1:5" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A72" s="20" t="s">
         <v>219</v>
       </c>
-      <c r="B69" s="7" t="s">
+      <c r="B72" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="C69" s="7" t="s">
+      <c r="C72" s="20" t="s">
         <v>220</v>
       </c>
-      <c r="E69" s="7" t="s">
+      <c r="E72" s="20" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="70" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="7" t="s">
+    <row r="73" spans="1:5" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A73" s="20" t="s">
         <v>205</v>
       </c>
-      <c r="B70" s="7" t="s">
+      <c r="B73" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="C70" s="7" t="s">
+      <c r="C73" s="20" t="s">
         <v>206</v>
       </c>
-      <c r="E70" s="7" t="s">
+      <c r="E73" s="20" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="71" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A71" s="7" t="s">
+    <row r="74" spans="1:5" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A74" s="20" t="s">
         <v>222</v>
       </c>
-      <c r="B71" s="7" t="s">
+      <c r="B74" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="C71" s="7" t="s">
+      <c r="C74" s="20" t="s">
         <v>223</v>
       </c>
-      <c r="E71" s="7" t="s">
+      <c r="E74" s="20" t="s">
         <v>207</v>
       </c>
     </row>
@@ -2894,7 +2985,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>228</v>
       </c>
     </row>

</xml_diff>